<commit_message>
Initial changes on 2021-08-26. Mostly complete Futures and Terms.
</commit_message>
<xml_diff>
--- a/er/images/RecommendationTable.xlsx
+++ b/er/images/RecommendationTable.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t>Providers</t>
   </si>
@@ -117,9 +117,6 @@
     <t>3D Buildings &amp; Models</t>
   </si>
   <si>
-    <t>Mixed testing results</t>
-  </si>
-  <si>
     <t>I3S</t>
   </si>
   <si>
@@ -132,7 +129,25 @@
     <t>USDZ</t>
   </si>
   <si>
-    <t>Potential OGC GeoVolumes API</t>
+    <t xml:space="preserve">  Compatible &amp; Sucessfully tested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mixed testing results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Unsucessfully tested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Potential OGC GeoVolumes API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Using OGC SensorThings API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Future Work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  via plugin</t>
   </si>
 </sst>
 </file>
@@ -350,23 +365,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -398,12 +404,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -439,6 +439,27 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,274 +788,274 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
     </row>
     <row r="4" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="D4" s="6"/>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="37"/>
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="1.35">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
+      <c r="E5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="19"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="38"/>
+      <c r="C6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
+      <c r="E6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="19"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
       <c r="K7" s="1"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
       <c r="K8" s="1"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="38"/>
+      <c r="C9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="17" t="s">
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="14" t="s">
         <v>12</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
       <c r="K10" s="1"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="38"/>
+      <c r="C11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="14"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="11"/>
       <c r="K11" s="1"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="1.35">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="16"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="1"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="39"/>
+      <c r="C13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
       <c r="K13" s="1"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
     </row>
     <row r="15" spans="2:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E15" s="20"/>
+      <c r="E15" s="15"/>
       <c r="G15" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E16" s="21"/>
+      <c r="E16" s="16"/>
       <c r="G16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="5:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E17" s="22"/>
+      <c r="E17" s="17"/>
       <c r="G17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="5:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E18" s="23"/>
+      <c r="E18" s="18"/>
       <c r="G18" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="5:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E19" s="24"/>
+      <c r="E19" s="19"/>
       <c r="G19" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="5:7" s="2" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="20" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -1042,7 +1063,7 @@
       </c>
     </row>
     <row r="21" spans="5:7" s="2" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E21" s="26"/>
+      <c r="E21" s="21"/>
       <c r="G21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1063,242 +1084,243 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="10" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
     </row>
     <row r="4" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="D4" s="6"/>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="37"/>
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="1.35">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="40"/>
+      <c r="C6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="19"/>
-      <c r="C6" s="12" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="1"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+    </row>
+    <row r="7" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="40"/>
+      <c r="C7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D7" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="1"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-    </row>
-    <row r="7" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="19"/>
-      <c r="C7" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="31" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="22"/>
+      <c r="J7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+    </row>
+    <row r="8" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="40"/>
+      <c r="C8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="27"/>
-      <c r="J7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-    </row>
-    <row r="8" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="12" t="s">
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="1"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+    </row>
+    <row r="9" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="1.35">
+      <c r="B9" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="1"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+    </row>
+    <row r="10" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="41"/>
+      <c r="C10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D10" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="1"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E12" s="29"/>
+      <c r="F12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="1"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-    </row>
-    <row r="9" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="1.35">
-      <c r="B9" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="1"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
-      <c r="C10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="1"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-    </row>
-    <row r="12" spans="2:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E12" s="34"/>
-      <c r="G12" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="13" spans="2:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E13" s="35"/>
-      <c r="G13" s="2" t="s">
-        <v>30</v>
+      <c r="E13" s="30"/>
+      <c r="F13" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="2:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E14" s="36"/>
-      <c r="G14" s="2" t="s">
-        <v>7</v>
+      <c r="E14" s="31"/>
+      <c r="F14" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="2:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E15" s="37"/>
-      <c r="G15" s="2" t="s">
-        <v>35</v>
+      <c r="E15" s="32"/>
+      <c r="F15" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E16" s="38"/>
-      <c r="G16" s="2" t="s">
-        <v>9</v>
+      <c r="E16" s="33"/>
+      <c r="F16" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="4:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E17" s="39"/>
-      <c r="G17" s="2" t="s">
-        <v>10</v>
+      <c r="E17" s="34"/>
+      <c r="F17" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="4:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E18" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>11</v>
+      <c r="E18" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="4:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>